<commit_message>
Changes to add google drive storage
</commit_message>
<xml_diff>
--- a/app/www/project_logbook.xlsx
+++ b/app/www/project_logbook.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -32,58 +32,19 @@
     <t xml:space="preserve">Survey_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Privacy_Options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other_Detail</t>
-  </si>
-  <si>
     <t xml:space="preserve">Study_Area</t>
   </si>
   <si>
     <t xml:space="preserve">Data_File</t>
   </si>
   <si>
-    <t xml:space="preserve">a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-11-08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cindy Hurtado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cindymeliza@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enterprise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multispecies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enterprise2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">proj</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Enterprise-2023-11-08.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enterprise2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enterprise2-2023-11-08.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Badger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">badger</t>
+    <t xml:space="preserve">2023-12-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test123-2023-12-06.csv</t>
   </si>
 </sst>
 </file>
@@ -440,171 +401,31 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added credentials to save files
</commit_message>
<xml_diff>
--- a/app/www/project_logbook.xlsx
+++ b/app/www/project_logbook.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -45,6 +45,21 @@
   </si>
   <si>
     <t xml:space="preserve">test123-2023-12-06.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">another</t>
+  </si>
+  <si>
+    <t xml:space="preserve">another-2023-12-06.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-12-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1-2023-12-08.csv</t>
   </si>
 </sst>
 </file>
@@ -428,6 +443,84 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>